<commit_message>
Updated RL Login credentials
Updated RL Login credentials
</commit_message>
<xml_diff>
--- a/AMCNetworks/src/main/java/com/amc/datasheets/AssestsIntegration.xlsx
+++ b/AMCNetworks/src/main/java/com/amc/datasheets/AssestsIntegration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="4215" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="4215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AssetInformation" sheetId="3" r:id="rId1"/>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>TestRailID</t>
-  </si>
-  <si>
-    <t>chandan.heralagi@amcnetworks.com</t>
-  </si>
-  <si>
-    <t>8KaRbijapur</t>
   </si>
   <si>
     <t>AssetType</t>
@@ -1156,6 +1150,12 @@
   </si>
   <si>
     <t>RLA219153</t>
+  </si>
+  <si>
+    <t>Chaitanya.Sunkara@amcnetworks.com</t>
+  </si>
+  <si>
+    <t>Speed!!0230</t>
   </si>
 </sst>
 </file>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,10 +1606,11 @@
     <col min="3" max="3" width="19" style="2" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.140625" style="2" collapsed="1"/>
-    <col min="8" max="8" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="13" width="9.140625" style="2" collapsed="1"/>
+    <col min="6" max="6" width="26.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="9.140625" style="2" collapsed="1"/>
     <col min="14" max="14" width="11.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="15" style="2" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1623,108 +1624,108 @@
   <sheetData>
     <row r="1" spans="1:22" ht="45">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="45">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J2" s="2">
         <v>2030</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="P2" s="5">
         <v>43586</v>
@@ -1733,390 +1734,390 @@
         <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="T2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:22" ht="45">
+    <row r="3" spans="1:22" ht="30">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2">
         <v>2030</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P3" s="5"/>
       <c r="R3" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="45">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="30">
       <c r="A4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2">
         <v>2030</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P4" s="5"/>
       <c r="R4" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="45">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="30">
       <c r="A5" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2">
         <v>2030</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P5" s="5"/>
       <c r="R5" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="45">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="30">
       <c r="A6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J6" s="2">
         <v>2030</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P6" s="5"/>
       <c r="R6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="45">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="30">
       <c r="A7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J7" s="2">
         <v>2030</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P7" s="5"/>
       <c r="R7" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="45">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="30">
       <c r="A8" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="2">
         <v>2030</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P8" s="5"/>
       <c r="R8" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="45">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="30">
       <c r="A9" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" s="2">
         <v>2030</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P9" s="5"/>
       <c r="R9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="45">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="30">
       <c r="A10" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J10" s="2">
         <v>2030</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P10" s="5"/>
       <c r="R10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="45">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="30">
       <c r="A11" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J11" s="2">
         <v>2030</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P11" s="5"/>
       <c r="R11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2129,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2149,10 +2150,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>358</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2171,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2196,7 +2197,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2210,13 +2211,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D3">
         <v>13884</v>
@@ -2224,7 +2225,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2238,7 +2239,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2252,7 +2253,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2266,7 +2267,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2280,7 +2281,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2294,7 +2295,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2308,7 +2309,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2322,7 +2323,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2336,7 +2337,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2350,7 +2351,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2364,7 +2365,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2378,7 +2379,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2392,7 +2393,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2406,7 +2407,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2420,13 +2421,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D18">
         <v>13855</v>
@@ -2434,7 +2435,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2448,7 +2449,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2462,7 +2463,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2476,7 +2477,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2490,7 +2491,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2504,7 +2505,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2518,7 +2519,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2532,7 +2533,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -2546,7 +2547,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2560,7 +2561,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -2574,7 +2575,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -2588,7 +2589,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -2602,7 +2603,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -2616,7 +2617,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -2630,13 +2631,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D33">
         <v>15331</v>
@@ -2644,7 +2645,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -2658,13 +2659,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D35">
         <v>13886</v>
@@ -2672,7 +2673,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -2686,7 +2687,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -2700,7 +2701,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -2714,7 +2715,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -2728,7 +2729,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -2742,7 +2743,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -2756,7 +2757,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2770,7 +2771,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -2784,7 +2785,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -2798,7 +2799,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -2812,7 +2813,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2826,7 +2827,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -2840,7 +2841,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -2854,7 +2855,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -2868,13 +2869,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B50">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D50">
         <v>15405</v>
@@ -2882,7 +2883,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2896,13 +2897,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D52">
         <v>13887</v>
@@ -2910,7 +2911,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -2924,7 +2925,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -2938,7 +2939,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -2952,7 +2953,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -2966,7 +2967,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -2980,7 +2981,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2994,7 +2995,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -3008,7 +3009,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -3022,7 +3023,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -3036,7 +3037,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -3050,7 +3051,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -3064,7 +3065,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -3078,7 +3079,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -3092,7 +3093,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B66">
         <v>4</v>
@@ -3106,13 +3107,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B67">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D67">
         <v>15466</v>
@@ -3120,7 +3121,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B68">
         <v>4</v>
@@ -3134,13 +3135,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B69">
         <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D69">
         <v>13888</v>
@@ -3148,7 +3149,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -3162,7 +3163,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -3176,7 +3177,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B72">
         <v>5</v>
@@ -3190,7 +3191,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -3204,7 +3205,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B74">
         <v>5</v>
@@ -3218,7 +3219,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B75">
         <v>5</v>
@@ -3232,7 +3233,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B76">
         <v>5</v>
@@ -3246,7 +3247,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B77">
         <v>5</v>
@@ -3260,7 +3261,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B78">
         <v>5</v>
@@ -3274,7 +3275,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B79">
         <v>5</v>
@@ -3288,7 +3289,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B80">
         <v>5</v>
@@ -3302,7 +3303,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B81">
         <v>5</v>
@@ -3316,7 +3317,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B82">
         <v>5</v>
@@ -3330,7 +3331,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B83">
         <v>5</v>
@@ -3344,13 +3345,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B84">
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D84">
         <v>15483</v>
@@ -3358,7 +3359,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B85">
         <v>5</v>
@@ -3372,13 +3373,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B86">
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D86">
         <v>13890</v>
@@ -3386,7 +3387,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B87">
         <v>6</v>
@@ -3400,7 +3401,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B88">
         <v>6</v>
@@ -3414,7 +3415,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B89">
         <v>6</v>
@@ -3428,7 +3429,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B90">
         <v>6</v>
@@ -3442,7 +3443,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B91">
         <v>6</v>
@@ -3456,7 +3457,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B92">
         <v>6</v>
@@ -3470,7 +3471,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -3484,7 +3485,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B94">
         <v>6</v>
@@ -3498,7 +3499,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B95">
         <v>6</v>
@@ -3512,7 +3513,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -3526,7 +3527,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B97">
         <v>6</v>
@@ -3540,7 +3541,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B98">
         <v>6</v>
@@ -3554,7 +3555,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B99">
         <v>6</v>
@@ -3568,7 +3569,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B100">
         <v>6</v>
@@ -3582,13 +3583,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B101">
         <v>6</v>
       </c>
       <c r="C101" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D101">
         <v>15517</v>
@@ -3596,7 +3597,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B102">
         <v>6</v>
@@ -3610,13 +3611,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B103">
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D103">
         <v>13889</v>
@@ -3624,7 +3625,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B104">
         <v>7</v>
@@ -3638,7 +3639,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B105">
         <v>7</v>
@@ -3652,7 +3653,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B106">
         <v>7</v>
@@ -3666,7 +3667,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B107">
         <v>7</v>
@@ -3680,7 +3681,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B108">
         <v>7</v>
@@ -3694,7 +3695,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B109">
         <v>7</v>
@@ -3708,7 +3709,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B110">
         <v>7</v>
@@ -3722,7 +3723,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B111">
         <v>7</v>
@@ -3736,7 +3737,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B112">
         <v>7</v>
@@ -3750,7 +3751,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B113">
         <v>7</v>
@@ -3764,7 +3765,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B114">
         <v>7</v>
@@ -3778,7 +3779,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B115">
         <v>7</v>
@@ -3792,7 +3793,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B116">
         <v>7</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B117">
         <v>7</v>
@@ -3820,13 +3821,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B118">
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D118">
         <v>15500</v>
@@ -3834,7 +3835,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B119">
         <v>7</v>
@@ -3848,13 +3849,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B120">
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D120">
         <v>13893</v>
@@ -3862,7 +3863,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B121">
         <v>8</v>
@@ -3876,7 +3877,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B122">
         <v>8</v>
@@ -3890,7 +3891,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B123">
         <v>8</v>
@@ -3904,7 +3905,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B124">
         <v>8</v>
@@ -3918,7 +3919,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B125">
         <v>8</v>
@@ -3932,7 +3933,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B126">
         <v>8</v>
@@ -3946,7 +3947,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B127">
         <v>8</v>
@@ -3960,7 +3961,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B128">
         <v>8</v>
@@ -3974,7 +3975,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B129">
         <v>8</v>
@@ -3988,7 +3989,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B130">
         <v>8</v>
@@ -4002,7 +4003,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B131">
         <v>8</v>
@@ -4016,7 +4017,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B132">
         <v>8</v>
@@ -4030,7 +4031,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B133">
         <v>8</v>
@@ -4044,7 +4045,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B134">
         <v>8</v>
@@ -4058,13 +4059,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B135">
         <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D135">
         <v>15540</v>
@@ -4072,7 +4073,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B136">
         <v>8</v>
@@ -4086,13 +4087,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B137">
         <v>9</v>
       </c>
       <c r="C137" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D137">
         <v>13891</v>
@@ -4100,7 +4101,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B138">
         <v>9</v>
@@ -4114,7 +4115,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B139">
         <v>9</v>
@@ -4128,7 +4129,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B140">
         <v>9</v>
@@ -4142,7 +4143,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B141">
         <v>9</v>
@@ -4156,7 +4157,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B142">
         <v>9</v>
@@ -4170,7 +4171,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B143">
         <v>9</v>
@@ -4184,7 +4185,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B144">
         <v>9</v>
@@ -4198,7 +4199,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B145">
         <v>9</v>
@@ -4212,7 +4213,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B146">
         <v>9</v>
@@ -4226,7 +4227,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B147">
         <v>9</v>
@@ -4240,7 +4241,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B148">
         <v>9</v>
@@ -4254,7 +4255,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B149">
         <v>9</v>
@@ -4268,7 +4269,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B150">
         <v>9</v>
@@ -4282,7 +4283,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B151">
         <v>9</v>
@@ -4296,13 +4297,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B152">
         <v>9</v>
       </c>
       <c r="C152" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D152">
         <v>15590</v>
@@ -4310,7 +4311,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B153">
         <v>9</v>
@@ -4324,13 +4325,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B154">
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D154">
         <v>13892</v>
@@ -4338,7 +4339,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B155">
         <v>10</v>
@@ -4352,7 +4353,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B156">
         <v>10</v>
@@ -4366,7 +4367,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B157">
         <v>10</v>
@@ -4380,7 +4381,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B158">
         <v>10</v>
@@ -4394,7 +4395,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B159">
         <v>10</v>
@@ -4408,7 +4409,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B160">
         <v>10</v>
@@ -4422,7 +4423,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B161">
         <v>10</v>
@@ -4436,7 +4437,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B162">
         <v>10</v>
@@ -4450,7 +4451,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B163">
         <v>10</v>
@@ -4464,7 +4465,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B164">
         <v>10</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B165">
         <v>10</v>
@@ -4492,7 +4493,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B166">
         <v>10</v>
@@ -4506,7 +4507,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B167">
         <v>10</v>
@@ -4520,7 +4521,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B168">
         <v>10</v>
@@ -4534,13 +4535,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B169">
         <v>10</v>
       </c>
       <c r="C169" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D169">
         <v>15557</v>
@@ -4548,7 +4549,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B170">
         <v>10</v>
@@ -4562,7 +4563,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -4596,10 +4597,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>3</v>
@@ -4607,13 +4608,13 @@
     </row>
     <row r="2" spans="1:3" ht="16.5">
       <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4634,7 +4635,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="409.5">
       <c r="A1" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -4662,82 +4663,82 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="48" customHeight="1">
       <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5">
       <c r="A3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5">
       <c r="A4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="F4" t="s">
         <v>60</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -4768,269 +4769,269 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
         <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
         <v>96</v>
-      </c>
-      <c r="C14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
         <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" t="s">
         <v>108</v>
-      </c>
-      <c r="C19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -5058,42 +5059,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30">
       <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="345">
       <c r="A2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>142</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -5122,148 +5123,148 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>